<commit_message>
Update a_score temporary views, templates
</commit_message>
<xml_diff>
--- a/a_score/data/prime_police_data.xlsx
+++ b/a_score/data/prime_police_data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\paedison3\a_score\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\paedison3\a_score\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E71A7F-FA2B-44B9-B662-117F3EB33F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29865509-3F12-4995-B032-EABC27550353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="624" xr2:uid="{FA0813FA-CB0F-4B59-8071-35577C31DB12}"/>
+    <workbookView xWindow="-27585" yWindow="9270" windowWidth="19005" windowHeight="16200" tabRatio="624" activeTab="1" xr2:uid="{FA0813FA-CB0F-4B59-8071-35577C31DB12}"/>
   </bookViews>
   <sheets>
     <sheet name="exam" sheetId="1" r:id="rId1"/>
+    <sheet name="정답" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -83,29 +84,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"hyeongsa":[2,1,2,4,2,1,2,2,4,3,2,1,2,2,2,1,2,2,4,1,1,1,3,2,4,4,1,4,3,4,3,2,2,3,2,3,1,3,4,1],"heonbeob":[3,1,1,2,4,1,2,4,1,4,4,2,3,3,1,4,2,3,4,4,3,3,2,2,4,4,4,1,2,4,4,2,3,2,3,3,1,4,1,3],"gyeongchal":[3,2,3,4,4,3,2,4,4,1,2,3,3,4,4,3,3,2,1,2,4,4,1,2,2,4,2,3,4,1,2,1,3,3,4,1,3,3,3,3],"beomjoe":[2,2,2,3,2,1,2,3,2,2,2,4,4,2,2,1,4,4,2,1,2,1,1,3,2,4,3,2,2,4,3,2,4,1,4,3,1,4,3,2],"minbeob":[2,1,2,3,4,1,1,2,1,3,3,3,4,4,2,4,3,4,3,3,3,4,2,3,2,2,4,1,4,1,4,3,1,1,3,2,2,3,2,4]}</t>
+    <t>{"hyeongsa": [1, 3, 4, 4, 4, 2, 3, 2, 4, 3, 2, 3, 2, 1, 2, 2, 3, 1, 4, 1, 3, 1, 3, 1, 1, 4, 4, 3, 4, 1, 4, 2, 3, 1, 2, 3, 4, 3, 2, 1],"heonbeob": [1, 4, 4, 3, 2, 2, 4, 2, 1, 4, 4, 2, 2, 1, 4, 4, 1, 2, 2, 1, 3, 3, 3, 4, 3, 1, 1, 4, 1, 3, 1, 2, 1, 4, 3, 3, 4, 4, 1, 3],"gyeongchal": [4, 4, 2, 2, 3, 4, 3, 2, 3, 2, 4, 4, 4, 3, 4, 4, 2, 2, 4, 3, 2, 4, 3, 1, 2, 4, 3, 3, 3, 3, 2, 4, 4, 2, 2, 3, 4, 4, 3, 3],"beomjoe": [2, 2, 1, 4, 4, 2, 1, 2, 4, 4, 1, 1, 1, 3, 3, 1, 1, 4, 4, 2, 3, 2, 2, 4, 3, 3, 1, 2, 2, 4, 2, 2, 4, 2, 2, 3, 3, 3, 1, 3],"minbeob": [4, 4, 3, 3, 4, 4, 1, 3, 3, 4, 3, 1, 2, 2, 3, 1, 1, 2, 3, 1, 1, 1, 3, 1, 4, 4, 3, 2, 4, 3, 2, 3, 2, 1, 2, 4, 1, 1, 2, 2],"haenghag": [4, 2, 3, 2, 2, 4, 3, 4, 1, 1, 3, 2, 2, 4, 3, 1, 4, 3, 3, 2, 3, 1, 1, 3, 4, 1, 4, 4, 4, 1, 2, 1, 1, 3, 4, 4, 3, 2, 1, 4]}</t>
   </si>
   <si>
-    <t>{"hyeongsa":[1,2,4,1,3,1,1,4,4,4,1,3,2,2,1,4,4,2,4,2,1,2,4,2,4,2,2,1,2,4,3,2,4,3,3,2,1,3,1,3],"heonbeob":[1,3,1,3,2,2,3,1,3,2,4,3,3,3,2,1,3,3,1,4,2,3,4,1,4,1,1,1,4,2,2,1,4,2,4,2,3,1,2,1],"gyeongchal":[4,2,3,4,1,2,4,4,3,4,2,4,2,4,4,1,3,1,2,1,3,2,3,1,4,4,3,3,2,1,1,2,1,2,4,1,2,1,1,2],"beomjoe":[3,3,4,2,4,4,4,1,4,3,3,1,3,4,3,3,1,4,2,2,2,2,3,3,1,4,2,3,3,1,3,3,4,2,3,2,2,2,2,2],"minbeob":[2,3,3,1,4,3,2,1,3,4,4,2,1,1,1,4,1,2,3,4,2,2,2,2,4,3,4,3,2,4,1,1,2,2,1,4,3,3,2,2]}</t>
+    <t>번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>{"hyeongsa":[4,2,4,1,2,3,4,4,3,2,2,2,4,3,4,4,3,3,4,3,2,2,4,1,3,1,3,3,3,2,3,4,3,1,2,4,1,4,3,2],"heonbeob":[3,3,4,2,3,4,2,3,3,3,4,2,3,1,2,4,3,1,2,2,4,3,4,2,3,1,1,2,4,4,3,1,4,1,3,2,4,4,2,4],"gyeongchal":[1,2,4,4,4,3,2,4,4,3,4,1,1,1,3,2,3,3,3,4,1,4,4,2,1,1,1,3,4,1,2,4,4,2,2,2,3,1,2,3],"beomjoe":[3,4,2,3,4,4,2,4,2,3,4,4,3,2,4,2,1,4,4,2,4,4,2,3,4,3,1,1,3,1,2,1,2,2,3,1,2,3,1,4],"minbeob":[1,4,2,3,4,4,3,2,1,3,2,4,1,2,3,2,2,1,1,3,3,3,2,3,2,4,2,3,2,2,3,1,1,3,1,1,3,3,1,1]}</t>
+    <t>형사법</t>
   </si>
   <si>
-    <t>{"hyeongsa":[3,2,2,2,4,1,3,2,3,4,4,1,4,3,4,2,3,3,1,2,2,2,4,2,1,1,4,2,3,4,2,3,1,1,2,2,4,2,4,3],"heonbeob":[4,4,4,2,2,1,3,2,2,4,4,3,4,4,3,1,4,4,3,2,3,2,4,3,2,4,4,1,2,4,2,2,3,2,4,4,1,4,3,2],"gyeongchal":[3,1,4,1,3,3,4,1,1,3,1,2,1,2,3,4,4,1,1,3,4,4,3,4,1,3,1,2,2,1,3,3,4,1,1,1,4,1,2,3],"beomjoe":[4,1,3,2,2,2,4,3,2,4,2,2,3,2,1,1,1,1,3,3,4,1,4,3,2,3,2,2,4,4,3,4,3,3,1,3,4,1,1,3],"minbeob":[2,2,4,2,3,1,4,3,1,1,3,3,4,3,2,4,3,2,1,4,3,2,1,4,3,2,2,4,1,2,3,1,3,1,3,2,2,1,3,4]}</t>
+    <t>헌법</t>
   </si>
   <si>
-    <t>{"hyeongsa":[2,3,2,2,3,1,4,3,3,3,4,1,3,2,3,2,2,4,4,2,3,3,1,2,3,2,3,3,1,4,2,2,2,1,4,4,3,3,4,4],"heonbeob":[4,1,3,1,3,1,2,3,4,1,4,3,2,3,4,4,1,2,4,3,2,4,1,3,1,2,2,3,3,1,2,1,2,1,3,1,1,3,3,2],"gyeongchal":[3,4,3,1,3,3,2,4,2,2,3,2,4,2,3,1,2,2,4,4,3,4,2,1,4,2,3,3,2,4,1,2,2,2,1,3,3,4,3,1],"beomjoe":[1,2,3,4,3,2,3,3,1,4,1,3,4,4,3,4,1,3,3,3,1,3,1,2,1,3,4,2,3,4,2,3,2,3,3,3,3,1,2,2],"minbeob":[4,3,4,2,2,2,1,1,3,2,2,3,1,2,4,4,3,2,4,2,4,2,2,2,1,2,2,1,3,4,2,4,1,4,4,4,4,2,1,4]}</t>
+    <t>경찰학</t>
   </si>
   <si>
-    <t>{"hyeongsa":[3,3,1,4,3,2,4,4,3,4,3,3,2,3,3,1,4,1,1,3,3,4,1,4,2,3,3,4,4,4,2,1,3,2,2,3,1,3,1,3],"heonbeob":[2,1,4,4,4,4,2,3,1,4,2,1,4,2,4,4,3,3,3,3,3,4,1,1,1,3,4,3,3,3,2,1,3,1,3,3,4,4,4,3],"gyeongchal":[3,1,1,2,4,2,1,4,2,2,3,3,4,4,2,3,1,1,1,4,3,2,2,1,1,4,4,2,2,3,1,4,1,1,1,3,2,2,3,1],"beomjoe":[2,2,3,2,2,3,2,1,2,1,4,3,2,4,1,2,3,4,1,2,3,4,2,1,2,4,4,2,3,1,2,2,2,2,2,1,2,1,4,1],"minbeob":[3,4,1,4,4,2,3,3,4,3,2,2,4,4,1,2,2,1,2,4,2,4,2,3,2,4,3,2,4,1,3,4,4,4,4,2,4,2,1,4]}</t>
+    <t>범죄학</t>
+  </si>
+  <si>
+    <t>민법총칙</t>
+  </si>
+  <si>
+    <t>행정학</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +136,12 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -146,22 +160,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="표준 2" xfId="1" xr:uid="{8CC101E0-19F4-46CD-9024-305764D1A8E0}"/>
+    <cellStyle name="표준 3" xfId="2" xr:uid="{69B41BEE-D254-462C-AC29-91B0BB9E249D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -473,11 +497,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1C590B-5E07-4E0D-9AB9-A615F59A5832}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -508,7 +532,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" cm="1">
-        <f t="array" ref="A2:A7">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
+        <f t="array" ref="A2">_xlfn.SEQUENCE(COUNTA(C:C)-1)</f>
         <v>1</v>
       </c>
       <c r="B2">
@@ -524,98 +548,976 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2025</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2025</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2025</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2025</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>2025</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:D11">
-    <sortCondition ref="C8:C11"/>
-    <sortCondition ref="D8:D11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:D6">
+    <sortCondition ref="C3:C6"/>
+    <sortCondition ref="D3:D6"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D348BE0-8638-45F8-91F5-259F06B21DBC}">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>4</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4</v>
+      </c>
+      <c r="E20" s="1">
+        <v>4</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+      <c r="G20" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>4</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>3</v>
+      </c>
+      <c r="F26" s="1">
+        <v>4</v>
+      </c>
+      <c r="G26" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>3</v>
+      </c>
+      <c r="G28" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>4</v>
+      </c>
+      <c r="G30" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2</v>
+      </c>
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>4</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>4</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2</v>
+      </c>
+      <c r="E36" s="1">
+        <v>2</v>
+      </c>
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+      <c r="G36" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1">
+        <v>3</v>
+      </c>
+      <c r="C37" s="1">
+        <v>3</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3</v>
+      </c>
+      <c r="F37" s="1">
+        <v>4</v>
+      </c>
+      <c r="G37" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4</v>
+      </c>
+      <c r="D38" s="1">
+        <v>4</v>
+      </c>
+      <c r="E38" s="1">
+        <v>3</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3</v>
+      </c>
+      <c r="C39" s="1">
+        <v>4</v>
+      </c>
+      <c r="D39" s="1">
+        <v>4</v>
+      </c>
+      <c r="E39" s="1">
+        <v>3</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>3</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>2</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1">
+        <v>3</v>
+      </c>
+      <c r="F41" s="1">
+        <v>2</v>
+      </c>
+      <c r="G41" s="2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>